<commit_message>
Refine PVS TV layout, gradients, and automation scripts
</commit_message>
<xml_diff>
--- a/PVS/Planned_qtys.xlsx
+++ b/PVS/Planned_qtys.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Logistics\4_BSA\9_Scripts_Reports\Daily_Production_IT\PVS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D128E0-A113-4E5B-BDBA-4FDC5AB1B91B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C05541C-9313-4C9A-AB7D-468958A7B0C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{86600EFC-FD9C-43BB-B6BA-9F2124CEAC73}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{86600EFC-FD9C-43BB-B6BA-9F2124CEAC73}"/>
   </bookViews>
   <sheets>
     <sheet name="Planned_qtys" sheetId="1" r:id="rId1"/>
@@ -2525,16 +2525,32 @@
           </cell>
           <cell r="CV7"/>
           <cell r="CW7"/>
-          <cell r="CX7"/>
-          <cell r="CY7"/>
-          <cell r="CZ7"/>
-          <cell r="DA7"/>
-          <cell r="DB7"/>
+          <cell r="CX7">
+            <v>596</v>
+          </cell>
+          <cell r="CY7">
+            <v>596</v>
+          </cell>
+          <cell r="CZ7">
+            <v>596</v>
+          </cell>
+          <cell r="DA7">
+            <v>596</v>
+          </cell>
+          <cell r="DB7">
+            <v>596</v>
+          </cell>
           <cell r="DC7"/>
           <cell r="DD7"/>
-          <cell r="DE7"/>
-          <cell r="DF7"/>
-          <cell r="DG7"/>
+          <cell r="DE7">
+            <v>472.6</v>
+          </cell>
+          <cell r="DF7">
+            <v>473</v>
+          </cell>
+          <cell r="DG7">
+            <v>473</v>
+          </cell>
           <cell r="DH7"/>
           <cell r="DI7"/>
           <cell r="DJ7"/>
@@ -2729,19 +2745,41 @@
           <cell r="CT8">
             <v>496</v>
           </cell>
-          <cell r="CU8"/>
-          <cell r="CV8"/>
+          <cell r="CU8">
+            <v>588</v>
+          </cell>
+          <cell r="CV8">
+            <v>0</v>
+          </cell>
           <cell r="CW8"/>
-          <cell r="CX8"/>
-          <cell r="CY8"/>
-          <cell r="CZ8"/>
-          <cell r="DA8"/>
-          <cell r="DB8"/>
-          <cell r="DC8"/>
+          <cell r="CX8">
+            <v>612</v>
+          </cell>
+          <cell r="CY8">
+            <v>596</v>
+          </cell>
+          <cell r="CZ8">
+            <v>680</v>
+          </cell>
+          <cell r="DA8">
+            <v>548</v>
+          </cell>
+          <cell r="DB8">
+            <v>440</v>
+          </cell>
+          <cell r="DC8">
+            <v>40</v>
+          </cell>
           <cell r="DD8"/>
-          <cell r="DE8"/>
-          <cell r="DF8"/>
-          <cell r="DG8"/>
+          <cell r="DE8">
+            <v>488</v>
+          </cell>
+          <cell r="DF8">
+            <v>456</v>
+          </cell>
+          <cell r="DG8">
+            <v>492</v>
+          </cell>
           <cell r="DH8"/>
           <cell r="DI8"/>
           <cell r="DJ8"/>
@@ -3128,16 +3166,32 @@
           </cell>
           <cell r="CV10"/>
           <cell r="CW10"/>
-          <cell r="CX10"/>
-          <cell r="CY10"/>
-          <cell r="CZ10"/>
-          <cell r="DA10"/>
-          <cell r="DB10"/>
+          <cell r="CX10">
+            <v>189</v>
+          </cell>
+          <cell r="CY10">
+            <v>189</v>
+          </cell>
+          <cell r="CZ10">
+            <v>189</v>
+          </cell>
+          <cell r="DA10">
+            <v>189</v>
+          </cell>
+          <cell r="DB10">
+            <v>189</v>
+          </cell>
           <cell r="DC10"/>
           <cell r="DD10"/>
-          <cell r="DE10"/>
-          <cell r="DF10"/>
-          <cell r="DG10"/>
+          <cell r="DE10">
+            <v>199.6</v>
+          </cell>
+          <cell r="DF10">
+            <v>200</v>
+          </cell>
+          <cell r="DG10">
+            <v>200</v>
+          </cell>
           <cell r="DH10"/>
           <cell r="DI10"/>
           <cell r="DJ10"/>
@@ -3332,19 +3386,41 @@
           <cell r="CT11">
             <v>110</v>
           </cell>
-          <cell r="CU11"/>
-          <cell r="CV11"/>
+          <cell r="CU11">
+            <v>110</v>
+          </cell>
+          <cell r="CV11">
+            <v>0</v>
+          </cell>
           <cell r="CW11"/>
-          <cell r="CX11"/>
-          <cell r="CY11"/>
-          <cell r="CZ11"/>
-          <cell r="DA11"/>
-          <cell r="DB11"/>
-          <cell r="DC11"/>
+          <cell r="CX11">
+            <v>162</v>
+          </cell>
+          <cell r="CY11">
+            <v>154</v>
+          </cell>
+          <cell r="CZ11">
+            <v>162</v>
+          </cell>
+          <cell r="DA11">
+            <v>198</v>
+          </cell>
+          <cell r="DB11">
+            <v>154</v>
+          </cell>
+          <cell r="DC11">
+            <v>0</v>
+          </cell>
           <cell r="DD11"/>
-          <cell r="DE11"/>
-          <cell r="DF11"/>
-          <cell r="DG11"/>
+          <cell r="DE11">
+            <v>186</v>
+          </cell>
+          <cell r="DF11">
+            <v>198</v>
+          </cell>
+          <cell r="DG11">
+            <v>230</v>
+          </cell>
           <cell r="DH11"/>
           <cell r="DI11"/>
           <cell r="DJ11"/>
@@ -3731,16 +3807,32 @@
           </cell>
           <cell r="CV13"/>
           <cell r="CW13"/>
-          <cell r="CX13"/>
-          <cell r="CY13"/>
-          <cell r="CZ13"/>
-          <cell r="DA13"/>
-          <cell r="DB13"/>
+          <cell r="CX13">
+            <v>393</v>
+          </cell>
+          <cell r="CY13">
+            <v>393</v>
+          </cell>
+          <cell r="CZ13">
+            <v>393</v>
+          </cell>
+          <cell r="DA13">
+            <v>393</v>
+          </cell>
+          <cell r="DB13">
+            <v>393</v>
+          </cell>
           <cell r="DC13"/>
           <cell r="DD13"/>
-          <cell r="DE13"/>
-          <cell r="DF13"/>
-          <cell r="DG13"/>
+          <cell r="DE13">
+            <v>393</v>
+          </cell>
+          <cell r="DF13">
+            <v>393</v>
+          </cell>
+          <cell r="DG13">
+            <v>393</v>
+          </cell>
           <cell r="DH13"/>
           <cell r="DI13"/>
           <cell r="DJ13"/>
@@ -3935,19 +4027,41 @@
           <cell r="CT14">
             <v>426</v>
           </cell>
-          <cell r="CU14"/>
-          <cell r="CV14"/>
+          <cell r="CU14">
+            <v>430</v>
+          </cell>
+          <cell r="CV14">
+            <v>0</v>
+          </cell>
           <cell r="CW14"/>
-          <cell r="CX14"/>
-          <cell r="CY14"/>
-          <cell r="CZ14"/>
-          <cell r="DA14"/>
-          <cell r="DB14"/>
-          <cell r="DC14"/>
+          <cell r="CX14">
+            <v>468</v>
+          </cell>
+          <cell r="CY14">
+            <v>426</v>
+          </cell>
+          <cell r="CZ14">
+            <v>274</v>
+          </cell>
+          <cell r="DA14">
+            <v>430</v>
+          </cell>
+          <cell r="DB14">
+            <v>156</v>
+          </cell>
+          <cell r="DC14">
+            <v>0</v>
+          </cell>
           <cell r="DD14"/>
-          <cell r="DE14"/>
-          <cell r="DF14"/>
-          <cell r="DG14"/>
+          <cell r="DE14">
+            <v>472</v>
+          </cell>
+          <cell r="DF14">
+            <v>426</v>
+          </cell>
+          <cell r="DG14">
+            <v>350</v>
+          </cell>
           <cell r="DH14"/>
           <cell r="DI14"/>
           <cell r="DJ14"/>
@@ -4334,16 +4448,32 @@
           </cell>
           <cell r="CV16"/>
           <cell r="CW16"/>
-          <cell r="CX16"/>
-          <cell r="CY16"/>
-          <cell r="CZ16"/>
-          <cell r="DA16"/>
-          <cell r="DB16"/>
+          <cell r="CX16">
+            <v>2621.6</v>
+          </cell>
+          <cell r="CY16">
+            <v>2622</v>
+          </cell>
+          <cell r="CZ16">
+            <v>2622</v>
+          </cell>
+          <cell r="DA16">
+            <v>2622</v>
+          </cell>
+          <cell r="DB16">
+            <v>2622</v>
+          </cell>
           <cell r="DC16"/>
           <cell r="DD16"/>
-          <cell r="DE16"/>
-          <cell r="DF16"/>
-          <cell r="DG16"/>
+          <cell r="DE16">
+            <v>2656.2</v>
+          </cell>
+          <cell r="DF16">
+            <v>2656</v>
+          </cell>
+          <cell r="DG16">
+            <v>2656</v>
+          </cell>
           <cell r="DH16"/>
           <cell r="DI16"/>
           <cell r="DJ16"/>
@@ -4538,19 +4668,41 @@
           <cell r="CT17">
             <v>1675</v>
           </cell>
-          <cell r="CU17"/>
-          <cell r="CV17"/>
+          <cell r="CU17">
+            <v>1550</v>
+          </cell>
+          <cell r="CV17">
+            <v>0</v>
+          </cell>
           <cell r="CW17"/>
-          <cell r="CX17"/>
-          <cell r="CY17"/>
-          <cell r="CZ17"/>
-          <cell r="DA17"/>
-          <cell r="DB17"/>
-          <cell r="DC17"/>
+          <cell r="CX17">
+            <v>1400</v>
+          </cell>
+          <cell r="CY17">
+            <v>1360</v>
+          </cell>
+          <cell r="CZ17">
+            <v>1285</v>
+          </cell>
+          <cell r="DA17">
+            <v>1515</v>
+          </cell>
+          <cell r="DB17">
+            <v>1350</v>
+          </cell>
+          <cell r="DC17">
+            <v>0</v>
+          </cell>
           <cell r="DD17"/>
-          <cell r="DE17"/>
-          <cell r="DF17"/>
-          <cell r="DG17"/>
+          <cell r="DE17">
+            <v>1525</v>
+          </cell>
+          <cell r="DF17">
+            <v>1425</v>
+          </cell>
+          <cell r="DG17">
+            <v>1660</v>
+          </cell>
           <cell r="DH17"/>
           <cell r="DI17"/>
           <cell r="DJ17"/>
@@ -4937,16 +5089,32 @@
           </cell>
           <cell r="CV19"/>
           <cell r="CW19"/>
-          <cell r="CX19"/>
-          <cell r="CY19"/>
-          <cell r="CZ19"/>
-          <cell r="DA19"/>
-          <cell r="DB19"/>
+          <cell r="CX19">
+            <v>1972.4</v>
+          </cell>
+          <cell r="CY19">
+            <v>1972</v>
+          </cell>
+          <cell r="CZ19">
+            <v>1972</v>
+          </cell>
+          <cell r="DA19">
+            <v>1972</v>
+          </cell>
+          <cell r="DB19">
+            <v>1972</v>
+          </cell>
           <cell r="DC19"/>
           <cell r="DD19"/>
-          <cell r="DE19"/>
-          <cell r="DF19"/>
-          <cell r="DG19"/>
+          <cell r="DE19">
+            <v>1985</v>
+          </cell>
+          <cell r="DF19">
+            <v>1985</v>
+          </cell>
+          <cell r="DG19">
+            <v>1985</v>
+          </cell>
           <cell r="DH19"/>
           <cell r="DI19"/>
           <cell r="DJ19"/>
@@ -5141,19 +5309,41 @@
           <cell r="CT20">
             <v>1890</v>
           </cell>
-          <cell r="CU20"/>
-          <cell r="CV20"/>
+          <cell r="CU20">
+            <v>1983</v>
+          </cell>
+          <cell r="CV20">
+            <v>0</v>
+          </cell>
           <cell r="CW20"/>
-          <cell r="CX20"/>
-          <cell r="CY20"/>
-          <cell r="CZ20"/>
-          <cell r="DA20"/>
-          <cell r="DB20"/>
-          <cell r="DC20"/>
+          <cell r="CX20">
+            <v>1923</v>
+          </cell>
+          <cell r="CY20">
+            <v>1866</v>
+          </cell>
+          <cell r="CZ20">
+            <v>1533</v>
+          </cell>
+          <cell r="DA20">
+            <v>1806</v>
+          </cell>
+          <cell r="DB20">
+            <v>1650</v>
+          </cell>
+          <cell r="DC20">
+            <v>63</v>
+          </cell>
           <cell r="DD20"/>
-          <cell r="DE20"/>
-          <cell r="DF20"/>
-          <cell r="DG20"/>
+          <cell r="DE20">
+            <v>1713</v>
+          </cell>
+          <cell r="DF20">
+            <v>1534</v>
+          </cell>
+          <cell r="DG20">
+            <v>2301</v>
+          </cell>
           <cell r="DH20"/>
           <cell r="DI20"/>
           <cell r="DJ20"/>
@@ -5540,16 +5730,32 @@
           </cell>
           <cell r="CV22"/>
           <cell r="CW22"/>
-          <cell r="CX22"/>
-          <cell r="CY22"/>
-          <cell r="CZ22"/>
-          <cell r="DA22"/>
-          <cell r="DB22"/>
+          <cell r="CX22">
+            <v>707</v>
+          </cell>
+          <cell r="CY22">
+            <v>707</v>
+          </cell>
+          <cell r="CZ22">
+            <v>707</v>
+          </cell>
+          <cell r="DA22">
+            <v>707</v>
+          </cell>
+          <cell r="DB22">
+            <v>707</v>
+          </cell>
           <cell r="DC22"/>
           <cell r="DD22"/>
-          <cell r="DE22"/>
-          <cell r="DF22"/>
-          <cell r="DG22"/>
+          <cell r="DE22">
+            <v>549</v>
+          </cell>
+          <cell r="DF22">
+            <v>549</v>
+          </cell>
+          <cell r="DG22">
+            <v>549</v>
+          </cell>
           <cell r="DH22"/>
           <cell r="DI22"/>
           <cell r="DJ22"/>
@@ -5744,19 +5950,41 @@
           <cell r="CT23">
             <v>366</v>
           </cell>
-          <cell r="CU23"/>
-          <cell r="CV23"/>
+          <cell r="CU23">
+            <v>270</v>
+          </cell>
+          <cell r="CV23">
+            <v>0</v>
+          </cell>
           <cell r="CW23"/>
-          <cell r="CX23"/>
-          <cell r="CY23"/>
-          <cell r="CZ23"/>
-          <cell r="DA23"/>
-          <cell r="DB23"/>
-          <cell r="DC23"/>
+          <cell r="CX23">
+            <v>612</v>
+          </cell>
+          <cell r="CY23">
+            <v>419</v>
+          </cell>
+          <cell r="CZ23">
+            <v>1284</v>
+          </cell>
+          <cell r="DA23">
+            <v>636</v>
+          </cell>
+          <cell r="DB23">
+            <v>188</v>
+          </cell>
+          <cell r="DC23">
+            <v>240</v>
+          </cell>
           <cell r="DD23"/>
-          <cell r="DE23"/>
-          <cell r="DF23"/>
-          <cell r="DG23"/>
+          <cell r="DE23">
+            <v>240</v>
+          </cell>
+          <cell r="DF23">
+            <v>336</v>
+          </cell>
+          <cell r="DG23">
+            <v>324</v>
+          </cell>
           <cell r="DH23"/>
           <cell r="DI23"/>
           <cell r="DJ23"/>
@@ -6143,16 +6371,32 @@
           </cell>
           <cell r="CV25"/>
           <cell r="CW25"/>
-          <cell r="CX25"/>
-          <cell r="CY25"/>
-          <cell r="CZ25"/>
-          <cell r="DA25"/>
-          <cell r="DB25"/>
+          <cell r="CX25">
+            <v>207.6</v>
+          </cell>
+          <cell r="CY25">
+            <v>208</v>
+          </cell>
+          <cell r="CZ25">
+            <v>208</v>
+          </cell>
+          <cell r="DA25">
+            <v>208</v>
+          </cell>
+          <cell r="DB25">
+            <v>208</v>
+          </cell>
           <cell r="DC25"/>
           <cell r="DD25"/>
-          <cell r="DE25"/>
-          <cell r="DF25"/>
-          <cell r="DG25"/>
+          <cell r="DE25">
+            <v>384.2</v>
+          </cell>
+          <cell r="DF25">
+            <v>384</v>
+          </cell>
+          <cell r="DG25">
+            <v>384</v>
+          </cell>
           <cell r="DH25"/>
           <cell r="DI25"/>
           <cell r="DJ25"/>
@@ -6347,19 +6591,41 @@
           <cell r="CT26">
             <v>210</v>
           </cell>
-          <cell r="CU26"/>
-          <cell r="CV26"/>
+          <cell r="CU26">
+            <v>200</v>
+          </cell>
+          <cell r="CV26">
+            <v>0</v>
+          </cell>
           <cell r="CW26"/>
-          <cell r="CX26"/>
-          <cell r="CY26"/>
-          <cell r="CZ26"/>
-          <cell r="DA26"/>
-          <cell r="DB26"/>
-          <cell r="DC26"/>
+          <cell r="CX26">
+            <v>132</v>
+          </cell>
+          <cell r="CY26">
+            <v>118</v>
+          </cell>
+          <cell r="CZ26">
+            <v>176</v>
+          </cell>
+          <cell r="DA26">
+            <v>198</v>
+          </cell>
+          <cell r="DB26">
+            <v>198</v>
+          </cell>
+          <cell r="DC26">
+            <v>0</v>
+          </cell>
           <cell r="DD26"/>
-          <cell r="DE26"/>
-          <cell r="DF26"/>
-          <cell r="DG26"/>
+          <cell r="DE26">
+            <v>442</v>
+          </cell>
+          <cell r="DF26">
+            <v>336</v>
+          </cell>
+          <cell r="DG26">
+            <v>206</v>
+          </cell>
           <cell r="DH26"/>
           <cell r="DI26"/>
           <cell r="DJ26"/>
@@ -6746,16 +7012,32 @@
           </cell>
           <cell r="CV28"/>
           <cell r="CW28"/>
-          <cell r="CX28"/>
-          <cell r="CY28"/>
-          <cell r="CZ28"/>
-          <cell r="DA28"/>
-          <cell r="DB28"/>
+          <cell r="CX28">
+            <v>1175.4000000000001</v>
+          </cell>
+          <cell r="CY28">
+            <v>1175</v>
+          </cell>
+          <cell r="CZ28">
+            <v>1175</v>
+          </cell>
+          <cell r="DA28">
+            <v>1175</v>
+          </cell>
+          <cell r="DB28">
+            <v>1175</v>
+          </cell>
           <cell r="DC28"/>
           <cell r="DD28"/>
-          <cell r="DE28"/>
-          <cell r="DF28"/>
-          <cell r="DG28"/>
+          <cell r="DE28">
+            <v>1185.2</v>
+          </cell>
+          <cell r="DF28">
+            <v>1185</v>
+          </cell>
+          <cell r="DG28">
+            <v>1185</v>
+          </cell>
           <cell r="DH28"/>
           <cell r="DI28"/>
           <cell r="DJ28"/>
@@ -6950,19 +7232,41 @@
           <cell r="CT29">
             <v>1240</v>
           </cell>
-          <cell r="CU29"/>
-          <cell r="CV29"/>
+          <cell r="CU29">
+            <v>1320</v>
+          </cell>
+          <cell r="CV29">
+            <v>0</v>
+          </cell>
           <cell r="CW29"/>
-          <cell r="CX29"/>
-          <cell r="CY29"/>
-          <cell r="CZ29"/>
-          <cell r="DA29"/>
-          <cell r="DB29"/>
-          <cell r="DC29"/>
+          <cell r="CX29">
+            <v>1182</v>
+          </cell>
+          <cell r="CY29">
+            <v>1338</v>
+          </cell>
+          <cell r="CZ29">
+            <v>1208</v>
+          </cell>
+          <cell r="DA29">
+            <v>1360</v>
+          </cell>
+          <cell r="DB29">
+            <v>1072</v>
+          </cell>
+          <cell r="DC29">
+            <v>0</v>
+          </cell>
           <cell r="DD29"/>
-          <cell r="DE29"/>
-          <cell r="DF29"/>
-          <cell r="DG29"/>
+          <cell r="DE29">
+            <v>1252</v>
+          </cell>
+          <cell r="DF29">
+            <v>1314</v>
+          </cell>
+          <cell r="DG29">
+            <v>1380</v>
+          </cell>
           <cell r="DH29"/>
           <cell r="DI29"/>
           <cell r="DJ29"/>
@@ -7349,16 +7653,32 @@
           </cell>
           <cell r="CV31"/>
           <cell r="CW31"/>
-          <cell r="CX31"/>
-          <cell r="CY31"/>
-          <cell r="CZ31"/>
-          <cell r="DA31"/>
-          <cell r="DB31"/>
+          <cell r="CX31">
+            <v>3505</v>
+          </cell>
+          <cell r="CY31">
+            <v>3505</v>
+          </cell>
+          <cell r="CZ31">
+            <v>3505</v>
+          </cell>
+          <cell r="DA31">
+            <v>3505</v>
+          </cell>
+          <cell r="DB31">
+            <v>3505</v>
+          </cell>
           <cell r="DC31"/>
           <cell r="DD31"/>
-          <cell r="DE31"/>
-          <cell r="DF31"/>
-          <cell r="DG31"/>
+          <cell r="DE31">
+            <v>3762.6</v>
+          </cell>
+          <cell r="DF31">
+            <v>3763</v>
+          </cell>
+          <cell r="DG31">
+            <v>3763</v>
+          </cell>
           <cell r="DH31"/>
           <cell r="DI31"/>
           <cell r="DJ31"/>
@@ -7553,19 +7873,41 @@
           <cell r="CT32">
             <v>3159</v>
           </cell>
-          <cell r="CU32"/>
-          <cell r="CV32"/>
+          <cell r="CU32">
+            <v>3358</v>
+          </cell>
+          <cell r="CV32">
+            <v>0</v>
+          </cell>
           <cell r="CW32"/>
-          <cell r="CX32"/>
-          <cell r="CY32"/>
-          <cell r="CZ32"/>
-          <cell r="DA32"/>
-          <cell r="DB32"/>
-          <cell r="DC32"/>
+          <cell r="CX32">
+            <v>3223</v>
+          </cell>
+          <cell r="CY32">
+            <v>3346</v>
+          </cell>
+          <cell r="CZ32">
+            <v>3543</v>
+          </cell>
+          <cell r="DA32">
+            <v>2835</v>
+          </cell>
+          <cell r="DB32">
+            <v>2867</v>
+          </cell>
+          <cell r="DC32">
+            <v>0</v>
+          </cell>
           <cell r="DD32"/>
-          <cell r="DE32"/>
-          <cell r="DF32"/>
-          <cell r="DG32"/>
+          <cell r="DE32">
+            <v>3025</v>
+          </cell>
+          <cell r="DF32">
+            <v>3475</v>
+          </cell>
+          <cell r="DG32">
+            <v>3750</v>
+          </cell>
           <cell r="DH32"/>
           <cell r="DI32"/>
           <cell r="DJ32"/>
@@ -7952,16 +8294,32 @@
           </cell>
           <cell r="CV34"/>
           <cell r="CW34"/>
-          <cell r="CX34"/>
-          <cell r="CY34"/>
-          <cell r="CZ34"/>
-          <cell r="DA34"/>
-          <cell r="DB34"/>
+          <cell r="CX34">
+            <v>299.8</v>
+          </cell>
+          <cell r="CY34">
+            <v>300</v>
+          </cell>
+          <cell r="CZ34">
+            <v>300</v>
+          </cell>
+          <cell r="DA34">
+            <v>300</v>
+          </cell>
+          <cell r="DB34">
+            <v>300</v>
+          </cell>
           <cell r="DC34"/>
           <cell r="DD34"/>
-          <cell r="DE34"/>
-          <cell r="DF34"/>
-          <cell r="DG34"/>
+          <cell r="DE34">
+            <v>299.8</v>
+          </cell>
+          <cell r="DF34">
+            <v>300</v>
+          </cell>
+          <cell r="DG34">
+            <v>300</v>
+          </cell>
           <cell r="DH34"/>
           <cell r="DI34"/>
           <cell r="DJ34"/>
@@ -8163,7 +8521,7 @@
             <v>315</v>
           </cell>
           <cell r="CU35">
-            <v>0</v>
+            <v>280</v>
           </cell>
           <cell r="CV35">
             <v>0</v>
@@ -8172,19 +8530,19 @@
             <v>0</v>
           </cell>
           <cell r="CX35">
-            <v>0</v>
+            <v>352</v>
           </cell>
           <cell r="CY35">
-            <v>0</v>
+            <v>325</v>
           </cell>
           <cell r="CZ35">
-            <v>0</v>
+            <v>285</v>
           </cell>
           <cell r="DA35">
-            <v>0</v>
+            <v>310</v>
           </cell>
           <cell r="DB35">
-            <v>0</v>
+            <v>310</v>
           </cell>
           <cell r="DC35">
             <v>0</v>
@@ -8193,13 +8551,13 @@
             <v>0</v>
           </cell>
           <cell r="DE35">
-            <v>0</v>
+            <v>325</v>
           </cell>
           <cell r="DF35">
-            <v>0</v>
+            <v>325</v>
           </cell>
           <cell r="DG35">
-            <v>0</v>
+            <v>325</v>
           </cell>
           <cell r="DH35">
             <v>0</v>
@@ -8905,16 +9263,32 @@
           </cell>
           <cell r="CV37"/>
           <cell r="CW37"/>
-          <cell r="CX37"/>
-          <cell r="CY37"/>
-          <cell r="CZ37"/>
-          <cell r="DA37"/>
-          <cell r="DB37"/>
+          <cell r="CX37">
+            <v>375.6</v>
+          </cell>
+          <cell r="CY37">
+            <v>376</v>
+          </cell>
+          <cell r="CZ37">
+            <v>376</v>
+          </cell>
+          <cell r="DA37">
+            <v>376</v>
+          </cell>
+          <cell r="DB37">
+            <v>376</v>
+          </cell>
           <cell r="DC37"/>
           <cell r="DD37"/>
-          <cell r="DE37"/>
-          <cell r="DF37"/>
-          <cell r="DG37"/>
+          <cell r="DE37">
+            <v>339</v>
+          </cell>
+          <cell r="DF37">
+            <v>219</v>
+          </cell>
+          <cell r="DG37">
+            <v>339</v>
+          </cell>
           <cell r="DH37"/>
           <cell r="DI37"/>
           <cell r="DJ37"/>
@@ -9116,7 +9490,7 @@
             <v>315</v>
           </cell>
           <cell r="CU38">
-            <v>0</v>
+            <v>383</v>
           </cell>
           <cell r="CV38">
             <v>0</v>
@@ -9125,19 +9499,19 @@
             <v>0</v>
           </cell>
           <cell r="CX38">
-            <v>0</v>
+            <v>390</v>
           </cell>
           <cell r="CY38">
-            <v>0</v>
+            <v>250</v>
           </cell>
           <cell r="CZ38">
-            <v>0</v>
+            <v>350.5</v>
           </cell>
           <cell r="DA38">
-            <v>0</v>
+            <v>325</v>
           </cell>
           <cell r="DB38">
-            <v>0</v>
+            <v>230</v>
           </cell>
           <cell r="DC38">
             <v>0</v>
@@ -9146,13 +9520,13 @@
             <v>0</v>
           </cell>
           <cell r="DE38">
-            <v>0</v>
+            <v>395</v>
           </cell>
           <cell r="DF38">
-            <v>0</v>
+            <v>206.5</v>
           </cell>
           <cell r="DG38">
-            <v>0</v>
+            <v>410</v>
           </cell>
           <cell r="DH38">
             <v>0</v>
@@ -9858,16 +10232,32 @@
           </cell>
           <cell r="CV40"/>
           <cell r="CW40"/>
-          <cell r="CX40"/>
-          <cell r="CY40"/>
-          <cell r="CZ40"/>
-          <cell r="DA40"/>
-          <cell r="DB40"/>
+          <cell r="CX40">
+            <v>730.4</v>
+          </cell>
+          <cell r="CY40">
+            <v>730</v>
+          </cell>
+          <cell r="CZ40">
+            <v>730</v>
+          </cell>
+          <cell r="DA40">
+            <v>730</v>
+          </cell>
+          <cell r="DB40">
+            <v>730</v>
+          </cell>
           <cell r="DC40"/>
           <cell r="DD40"/>
-          <cell r="DE40"/>
-          <cell r="DF40"/>
-          <cell r="DG40"/>
+          <cell r="DE40">
+            <v>730.4</v>
+          </cell>
+          <cell r="DF40">
+            <v>730</v>
+          </cell>
+          <cell r="DG40">
+            <v>730</v>
+          </cell>
           <cell r="DH40"/>
           <cell r="DI40"/>
           <cell r="DJ40"/>
@@ -10069,7 +10459,7 @@
             <v>714</v>
           </cell>
           <cell r="CU41">
-            <v>0</v>
+            <v>708</v>
           </cell>
           <cell r="CV41">
             <v>0</v>
@@ -10078,19 +10468,19 @@
             <v>0</v>
           </cell>
           <cell r="CX41">
-            <v>0</v>
+            <v>750</v>
           </cell>
           <cell r="CY41">
-            <v>0</v>
+            <v>738</v>
           </cell>
           <cell r="CZ41">
-            <v>0</v>
+            <v>699</v>
           </cell>
           <cell r="DA41">
-            <v>0</v>
+            <v>672</v>
           </cell>
           <cell r="DB41">
-            <v>0</v>
+            <v>528</v>
           </cell>
           <cell r="DC41">
             <v>0</v>
@@ -10099,13 +10489,13 @@
             <v>0</v>
           </cell>
           <cell r="DE41">
-            <v>0</v>
+            <v>714</v>
           </cell>
           <cell r="DF41">
-            <v>0</v>
+            <v>673</v>
           </cell>
           <cell r="DG41">
-            <v>0</v>
+            <v>693</v>
           </cell>
           <cell r="DH41">
             <v>0</v>
@@ -10811,16 +11201,32 @@
           </cell>
           <cell r="CV43"/>
           <cell r="CW43"/>
-          <cell r="CX43"/>
-          <cell r="CY43"/>
-          <cell r="CZ43"/>
-          <cell r="DA43"/>
-          <cell r="DB43"/>
+          <cell r="CX43">
+            <v>0</v>
+          </cell>
+          <cell r="CY43">
+            <v>0</v>
+          </cell>
+          <cell r="CZ43">
+            <v>0</v>
+          </cell>
+          <cell r="DA43">
+            <v>0</v>
+          </cell>
+          <cell r="DB43">
+            <v>0</v>
+          </cell>
           <cell r="DC43"/>
           <cell r="DD43"/>
-          <cell r="DE43"/>
-          <cell r="DF43"/>
-          <cell r="DG43"/>
+          <cell r="DE43">
+            <v>0</v>
+          </cell>
+          <cell r="DF43">
+            <v>0</v>
+          </cell>
+          <cell r="DG43">
+            <v>0</v>
+          </cell>
           <cell r="DH43"/>
           <cell r="DI43"/>
           <cell r="DJ43"/>
@@ -11764,16 +12170,32 @@
           </cell>
           <cell r="CV46"/>
           <cell r="CW46"/>
-          <cell r="CX46"/>
-          <cell r="CY46"/>
-          <cell r="CZ46"/>
-          <cell r="DA46"/>
-          <cell r="DB46"/>
+          <cell r="CX46">
+            <v>18</v>
+          </cell>
+          <cell r="CY46">
+            <v>18</v>
+          </cell>
+          <cell r="CZ46">
+            <v>18</v>
+          </cell>
+          <cell r="DA46">
+            <v>18</v>
+          </cell>
+          <cell r="DB46">
+            <v>18</v>
+          </cell>
           <cell r="DC46"/>
           <cell r="DD46"/>
-          <cell r="DE46"/>
-          <cell r="DF46"/>
-          <cell r="DG46"/>
+          <cell r="DE46">
+            <v>21.6</v>
+          </cell>
+          <cell r="DF46">
+            <v>22</v>
+          </cell>
+          <cell r="DG46">
+            <v>22</v>
+          </cell>
           <cell r="DH46"/>
           <cell r="DI46"/>
           <cell r="DJ46"/>
@@ -11987,16 +12409,16 @@
             <v>0</v>
           </cell>
           <cell r="CY47">
-            <v>0</v>
+            <v>15</v>
           </cell>
           <cell r="CZ47">
-            <v>0</v>
+            <v>10</v>
           </cell>
           <cell r="DA47">
-            <v>0</v>
+            <v>20</v>
           </cell>
           <cell r="DB47">
-            <v>0</v>
+            <v>15</v>
           </cell>
           <cell r="DC47">
             <v>0</v>
@@ -12005,13 +12427,13 @@
             <v>0</v>
           </cell>
           <cell r="DE47">
-            <v>0</v>
+            <v>20</v>
           </cell>
           <cell r="DF47">
-            <v>0</v>
+            <v>29.5</v>
           </cell>
           <cell r="DG47">
-            <v>0</v>
+            <v>22.5</v>
           </cell>
           <cell r="DH47">
             <v>0</v>
@@ -12717,16 +13139,32 @@
           </cell>
           <cell r="CV49"/>
           <cell r="CW49"/>
-          <cell r="CX49"/>
-          <cell r="CY49"/>
-          <cell r="CZ49"/>
-          <cell r="DA49"/>
-          <cell r="DB49"/>
+          <cell r="CX49">
+            <v>617.6</v>
+          </cell>
+          <cell r="CY49">
+            <v>618</v>
+          </cell>
+          <cell r="CZ49">
+            <v>618</v>
+          </cell>
+          <cell r="DA49">
+            <v>618</v>
+          </cell>
+          <cell r="DB49">
+            <v>618</v>
+          </cell>
           <cell r="DC49"/>
           <cell r="DD49"/>
-          <cell r="DE49"/>
-          <cell r="DF49"/>
-          <cell r="DG49"/>
+          <cell r="DE49">
+            <v>529.4</v>
+          </cell>
+          <cell r="DF49">
+            <v>529</v>
+          </cell>
+          <cell r="DG49">
+            <v>529</v>
+          </cell>
           <cell r="DH49"/>
           <cell r="DI49"/>
           <cell r="DJ49"/>
@@ -12921,19 +13359,41 @@
           <cell r="CT50">
             <v>500</v>
           </cell>
-          <cell r="CU50"/>
-          <cell r="CV50"/>
+          <cell r="CU50">
+            <v>400</v>
+          </cell>
+          <cell r="CV50">
+            <v>0</v>
+          </cell>
           <cell r="CW50"/>
-          <cell r="CX50"/>
-          <cell r="CY50"/>
-          <cell r="CZ50"/>
-          <cell r="DA50"/>
-          <cell r="DB50"/>
-          <cell r="DC50"/>
+          <cell r="CX50">
+            <v>600</v>
+          </cell>
+          <cell r="CY50">
+            <v>400</v>
+          </cell>
+          <cell r="CZ50">
+            <v>400</v>
+          </cell>
+          <cell r="DA50">
+            <v>400</v>
+          </cell>
+          <cell r="DB50">
+            <v>300</v>
+          </cell>
+          <cell r="DC50">
+            <v>0</v>
+          </cell>
           <cell r="DD50"/>
-          <cell r="DE50"/>
-          <cell r="DF50"/>
-          <cell r="DG50"/>
+          <cell r="DE50">
+            <v>400</v>
+          </cell>
+          <cell r="DF50">
+            <v>400</v>
+          </cell>
+          <cell r="DG50">
+            <v>400</v>
+          </cell>
           <cell r="DH50"/>
           <cell r="DI50"/>
           <cell r="DJ50"/>
@@ -13320,16 +13780,32 @@
           </cell>
           <cell r="CV52"/>
           <cell r="CW52"/>
-          <cell r="CX52"/>
-          <cell r="CY52"/>
-          <cell r="CZ52"/>
-          <cell r="DA52"/>
-          <cell r="DB52"/>
+          <cell r="CX52">
+            <v>3997.8</v>
+          </cell>
+          <cell r="CY52">
+            <v>3998</v>
+          </cell>
+          <cell r="CZ52">
+            <v>3998</v>
+          </cell>
+          <cell r="DA52">
+            <v>3998</v>
+          </cell>
+          <cell r="DB52">
+            <v>3998</v>
+          </cell>
           <cell r="DC52"/>
           <cell r="DD52"/>
-          <cell r="DE52"/>
-          <cell r="DF52"/>
-          <cell r="DG52"/>
+          <cell r="DE52">
+            <v>3997.8</v>
+          </cell>
+          <cell r="DF52">
+            <v>3998</v>
+          </cell>
+          <cell r="DG52">
+            <v>3998</v>
+          </cell>
           <cell r="DH52"/>
           <cell r="DI52"/>
           <cell r="DJ52"/>
@@ -13524,19 +14000,41 @@
           <cell r="CT53">
             <v>4747</v>
           </cell>
-          <cell r="CU53"/>
-          <cell r="CV53"/>
+          <cell r="CU53">
+            <v>5059</v>
+          </cell>
+          <cell r="CV53">
+            <v>105</v>
+          </cell>
           <cell r="CW53"/>
-          <cell r="CX53"/>
-          <cell r="CY53"/>
-          <cell r="CZ53"/>
-          <cell r="DA53"/>
-          <cell r="DB53"/>
-          <cell r="DC53"/>
+          <cell r="CX53">
+            <v>4327</v>
+          </cell>
+          <cell r="CY53">
+            <v>4920</v>
+          </cell>
+          <cell r="CZ53">
+            <v>4747</v>
+          </cell>
+          <cell r="DA53">
+            <v>5232</v>
+          </cell>
+          <cell r="DB53">
+            <v>4885</v>
+          </cell>
+          <cell r="DC53">
+            <v>205</v>
+          </cell>
           <cell r="DD53"/>
-          <cell r="DE53"/>
-          <cell r="DF53"/>
-          <cell r="DG53"/>
+          <cell r="DE53">
+            <v>4329</v>
+          </cell>
+          <cell r="DF53">
+            <v>4824</v>
+          </cell>
+          <cell r="DG53">
+            <v>4533</v>
+          </cell>
           <cell r="DH53"/>
           <cell r="DI53"/>
           <cell r="DJ53"/>
@@ -13923,16 +14421,32 @@
           </cell>
           <cell r="CV55"/>
           <cell r="CW55"/>
-          <cell r="CX55"/>
-          <cell r="CY55"/>
-          <cell r="CZ55"/>
-          <cell r="DA55"/>
-          <cell r="DB55"/>
+          <cell r="CX55">
+            <v>912.8</v>
+          </cell>
+          <cell r="CY55">
+            <v>1172.8</v>
+          </cell>
+          <cell r="CZ55">
+            <v>1173</v>
+          </cell>
+          <cell r="DA55">
+            <v>1173</v>
+          </cell>
+          <cell r="DB55">
+            <v>1173</v>
+          </cell>
           <cell r="DC55"/>
           <cell r="DD55"/>
-          <cell r="DE55"/>
-          <cell r="DF55"/>
-          <cell r="DG55"/>
+          <cell r="DE55">
+            <v>1172.8</v>
+          </cell>
+          <cell r="DF55">
+            <v>1173</v>
+          </cell>
+          <cell r="DG55">
+            <v>1173</v>
+          </cell>
           <cell r="DH55"/>
           <cell r="DI55"/>
           <cell r="DJ55"/>
@@ -14127,19 +14641,41 @@
           <cell r="CT56">
             <v>1026</v>
           </cell>
-          <cell r="CU56"/>
-          <cell r="CV56"/>
+          <cell r="CU56">
+            <v>828</v>
+          </cell>
+          <cell r="CV56">
+            <v>0</v>
+          </cell>
           <cell r="CW56"/>
-          <cell r="CX56"/>
-          <cell r="CY56"/>
-          <cell r="CZ56"/>
-          <cell r="DA56"/>
-          <cell r="DB56"/>
-          <cell r="DC56"/>
+          <cell r="CX56">
+            <v>888</v>
+          </cell>
+          <cell r="CY56">
+            <v>1182</v>
+          </cell>
+          <cell r="CZ56">
+            <v>1188</v>
+          </cell>
+          <cell r="DA56">
+            <v>846</v>
+          </cell>
+          <cell r="DB56">
+            <v>1158</v>
+          </cell>
+          <cell r="DC56">
+            <v>126</v>
+          </cell>
           <cell r="DD56"/>
-          <cell r="DE56"/>
-          <cell r="DF56"/>
-          <cell r="DG56"/>
+          <cell r="DE56">
+            <v>1050</v>
+          </cell>
+          <cell r="DF56">
+            <v>1056</v>
+          </cell>
+          <cell r="DG56">
+            <v>1008</v>
+          </cell>
           <cell r="DH56"/>
           <cell r="DI56"/>
           <cell r="DJ56"/>
@@ -14526,16 +15062,32 @@
           </cell>
           <cell r="CV58"/>
           <cell r="CW58"/>
-          <cell r="CX58"/>
-          <cell r="CY58"/>
-          <cell r="CZ58"/>
-          <cell r="DA58"/>
-          <cell r="DB58"/>
+          <cell r="CX58">
+            <v>218.6</v>
+          </cell>
+          <cell r="CY58">
+            <v>219</v>
+          </cell>
+          <cell r="CZ58">
+            <v>219</v>
+          </cell>
+          <cell r="DA58">
+            <v>219</v>
+          </cell>
+          <cell r="DB58">
+            <v>219</v>
+          </cell>
           <cell r="DC58"/>
           <cell r="DD58"/>
-          <cell r="DE58"/>
-          <cell r="DF58"/>
-          <cell r="DG58"/>
+          <cell r="DE58">
+            <v>424.2</v>
+          </cell>
+          <cell r="DF58">
+            <v>424</v>
+          </cell>
+          <cell r="DG58">
+            <v>424</v>
+          </cell>
           <cell r="DH58"/>
           <cell r="DI58"/>
           <cell r="DJ58"/>
@@ -14730,19 +15282,41 @@
           <cell r="CT59">
             <v>156</v>
           </cell>
-          <cell r="CU59"/>
-          <cell r="CV59"/>
+          <cell r="CU59">
+            <v>330</v>
+          </cell>
+          <cell r="CV59">
+            <v>0</v>
+          </cell>
           <cell r="CW59"/>
-          <cell r="CX59"/>
-          <cell r="CY59"/>
-          <cell r="CZ59"/>
-          <cell r="DA59"/>
-          <cell r="DB59"/>
-          <cell r="DC59"/>
+          <cell r="CX59">
+            <v>276</v>
+          </cell>
+          <cell r="CY59">
+            <v>232</v>
+          </cell>
+          <cell r="CZ59">
+            <v>198</v>
+          </cell>
+          <cell r="DA59">
+            <v>198</v>
+          </cell>
+          <cell r="DB59">
+            <v>264</v>
+          </cell>
+          <cell r="DC59">
+            <v>0</v>
+          </cell>
           <cell r="DD59"/>
-          <cell r="DE59"/>
-          <cell r="DF59"/>
-          <cell r="DG59"/>
+          <cell r="DE59">
+            <v>354</v>
+          </cell>
+          <cell r="DF59">
+            <v>432</v>
+          </cell>
+          <cell r="DG59">
+            <v>342</v>
+          </cell>
           <cell r="DH59"/>
           <cell r="DI59"/>
           <cell r="DJ59"/>
@@ -15129,16 +15703,32 @@
           </cell>
           <cell r="CV61"/>
           <cell r="CW61"/>
-          <cell r="CX61"/>
-          <cell r="CY61"/>
-          <cell r="CZ61"/>
-          <cell r="DA61"/>
-          <cell r="DB61"/>
+          <cell r="CX61">
+            <v>407.8</v>
+          </cell>
+          <cell r="CY61">
+            <v>408</v>
+          </cell>
+          <cell r="CZ61">
+            <v>408</v>
+          </cell>
+          <cell r="DA61">
+            <v>408</v>
+          </cell>
+          <cell r="DB61">
+            <v>408</v>
+          </cell>
           <cell r="DC61"/>
           <cell r="DD61"/>
-          <cell r="DE61"/>
-          <cell r="DF61"/>
-          <cell r="DG61"/>
+          <cell r="DE61">
+            <v>407.8</v>
+          </cell>
+          <cell r="DF61">
+            <v>408</v>
+          </cell>
+          <cell r="DG61">
+            <v>408</v>
+          </cell>
           <cell r="DH61"/>
           <cell r="DI61"/>
           <cell r="DJ61"/>
@@ -15333,19 +15923,41 @@
           <cell r="CT62">
             <v>324</v>
           </cell>
-          <cell r="CU62"/>
-          <cell r="CV62"/>
+          <cell r="CU62">
+            <v>240</v>
+          </cell>
+          <cell r="CV62">
+            <v>0</v>
+          </cell>
           <cell r="CW62"/>
-          <cell r="CX62"/>
-          <cell r="CY62"/>
-          <cell r="CZ62"/>
-          <cell r="DA62"/>
-          <cell r="DB62"/>
-          <cell r="DC62"/>
+          <cell r="CX62">
+            <v>408</v>
+          </cell>
+          <cell r="CY62">
+            <v>444</v>
+          </cell>
+          <cell r="CZ62">
+            <v>324</v>
+          </cell>
+          <cell r="DA62">
+            <v>384</v>
+          </cell>
+          <cell r="DB62">
+            <v>300</v>
+          </cell>
+          <cell r="DC62">
+            <v>180</v>
+          </cell>
           <cell r="DD62"/>
-          <cell r="DE62"/>
-          <cell r="DF62"/>
-          <cell r="DG62"/>
+          <cell r="DE62">
+            <v>120</v>
+          </cell>
+          <cell r="DF62">
+            <v>360</v>
+          </cell>
+          <cell r="DG62">
+            <v>612</v>
+          </cell>
           <cell r="DH62"/>
           <cell r="DI62"/>
           <cell r="DJ62"/>
@@ -15732,16 +16344,32 @@
           </cell>
           <cell r="CV64"/>
           <cell r="CW64"/>
-          <cell r="CX64"/>
-          <cell r="CY64"/>
-          <cell r="CZ64"/>
-          <cell r="DA64"/>
-          <cell r="DB64"/>
+          <cell r="CX64">
+            <v>203.2</v>
+          </cell>
+          <cell r="CY64">
+            <v>203</v>
+          </cell>
+          <cell r="CZ64">
+            <v>203</v>
+          </cell>
+          <cell r="DA64">
+            <v>203</v>
+          </cell>
+          <cell r="DB64">
+            <v>203</v>
+          </cell>
           <cell r="DC64"/>
           <cell r="DD64"/>
-          <cell r="DE64"/>
-          <cell r="DF64"/>
-          <cell r="DG64"/>
+          <cell r="DE64">
+            <v>304.8</v>
+          </cell>
+          <cell r="DF64">
+            <v>305</v>
+          </cell>
+          <cell r="DG64">
+            <v>305</v>
+          </cell>
           <cell r="DH64"/>
           <cell r="DI64"/>
           <cell r="DJ64"/>
@@ -15936,19 +16564,41 @@
           <cell r="CT65">
             <v>192</v>
           </cell>
-          <cell r="CU65"/>
-          <cell r="CV65"/>
+          <cell r="CU65">
+            <v>128</v>
+          </cell>
+          <cell r="CV65">
+            <v>0</v>
+          </cell>
           <cell r="CW65"/>
-          <cell r="CX65"/>
-          <cell r="CY65"/>
-          <cell r="CZ65"/>
-          <cell r="DA65"/>
-          <cell r="DB65"/>
-          <cell r="DC65"/>
+          <cell r="CX65">
+            <v>256</v>
+          </cell>
+          <cell r="CY65">
+            <v>0</v>
+          </cell>
+          <cell r="CZ65">
+            <v>256</v>
+          </cell>
+          <cell r="DA65">
+            <v>411</v>
+          </cell>
+          <cell r="DB65">
+            <v>256</v>
+          </cell>
+          <cell r="DC65">
+            <v>0</v>
+          </cell>
           <cell r="DD65"/>
-          <cell r="DE65"/>
-          <cell r="DF65"/>
-          <cell r="DG65"/>
+          <cell r="DE65">
+            <v>192</v>
+          </cell>
+          <cell r="DF65">
+            <v>320</v>
+          </cell>
+          <cell r="DG65">
+            <v>128</v>
+          </cell>
           <cell r="DH65"/>
           <cell r="DI65"/>
           <cell r="DJ65"/>
@@ -16335,16 +16985,32 @@
           </cell>
           <cell r="CV67"/>
           <cell r="CW67"/>
-          <cell r="CX67"/>
-          <cell r="CY67"/>
-          <cell r="CZ67"/>
-          <cell r="DA67"/>
-          <cell r="DB67"/>
+          <cell r="CX67">
+            <v>3603.6000000000004</v>
+          </cell>
+          <cell r="CY67">
+            <v>4113.6000000000004</v>
+          </cell>
+          <cell r="CZ67">
+            <v>4114</v>
+          </cell>
+          <cell r="DA67">
+            <v>4114</v>
+          </cell>
+          <cell r="DB67">
+            <v>4114</v>
+          </cell>
           <cell r="DC67"/>
           <cell r="DD67"/>
-          <cell r="DE67"/>
-          <cell r="DF67"/>
-          <cell r="DG67"/>
+          <cell r="DE67">
+            <v>4198</v>
+          </cell>
+          <cell r="DF67">
+            <v>4198</v>
+          </cell>
+          <cell r="DG67">
+            <v>4198</v>
+          </cell>
           <cell r="DH67"/>
           <cell r="DI67"/>
           <cell r="DJ67"/>
@@ -16539,19 +17205,41 @@
           <cell r="CT68">
             <v>3407</v>
           </cell>
-          <cell r="CU68"/>
-          <cell r="CV68"/>
+          <cell r="CU68">
+            <v>4009</v>
+          </cell>
+          <cell r="CV68">
+            <v>0</v>
+          </cell>
           <cell r="CW68"/>
-          <cell r="CX68"/>
-          <cell r="CY68"/>
-          <cell r="CZ68"/>
-          <cell r="DA68"/>
-          <cell r="DB68"/>
-          <cell r="DC68"/>
+          <cell r="CX68">
+            <v>3362</v>
+          </cell>
+          <cell r="CY68">
+            <v>3871</v>
+          </cell>
+          <cell r="CZ68">
+            <v>3797</v>
+          </cell>
+          <cell r="DA68">
+            <v>3820</v>
+          </cell>
+          <cell r="DB68">
+            <v>3319</v>
+          </cell>
+          <cell r="DC68">
+            <v>0</v>
+          </cell>
           <cell r="DD68"/>
-          <cell r="DE68"/>
-          <cell r="DF68"/>
-          <cell r="DG68"/>
+          <cell r="DE68">
+            <v>4208</v>
+          </cell>
+          <cell r="DF68">
+            <v>3655</v>
+          </cell>
+          <cell r="DG68">
+            <v>4070</v>
+          </cell>
           <cell r="DH68"/>
           <cell r="DI68"/>
           <cell r="DJ68"/>
@@ -17905,19 +18593,19 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>596</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>596</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>596</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>596</v>
       </c>
       <c r="T2">
-        <v>0</v>
+        <v>596</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -17926,13 +18614,13 @@
         <v>0</v>
       </c>
       <c r="W2">
-        <v>0</v>
+        <v>473</v>
       </c>
       <c r="X2">
-        <v>0</v>
+        <v>473</v>
       </c>
       <c r="Y2">
-        <v>0</v>
+        <v>473</v>
       </c>
       <c r="Z2">
         <v>0</v>
@@ -18459,19 +19147,19 @@
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>189</v>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <v>189</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>189</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <v>189</v>
       </c>
       <c r="T3">
-        <v>0</v>
+        <v>189</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -18480,13 +19168,13 @@
         <v>0</v>
       </c>
       <c r="W3">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="X3">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="Y3">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="Z3">
         <v>0</v>
@@ -19013,19 +19701,19 @@
         <v>0</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>393</v>
       </c>
       <c r="Q4">
-        <v>0</v>
+        <v>393</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>393</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>393</v>
       </c>
       <c r="T4">
-        <v>0</v>
+        <v>393</v>
       </c>
       <c r="U4">
         <v>0</v>
@@ -19034,13 +19722,13 @@
         <v>0</v>
       </c>
       <c r="W4">
-        <v>0</v>
+        <v>393</v>
       </c>
       <c r="X4">
-        <v>0</v>
+        <v>393</v>
       </c>
       <c r="Y4">
-        <v>0</v>
+        <v>393</v>
       </c>
       <c r="Z4">
         <v>0</v>
@@ -19567,19 +20255,19 @@
         <v>0</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>2622</v>
       </c>
       <c r="Q5">
-        <v>0</v>
+        <v>2622</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>2622</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <v>2622</v>
       </c>
       <c r="T5">
-        <v>0</v>
+        <v>2622</v>
       </c>
       <c r="U5">
         <v>0</v>
@@ -19588,13 +20276,13 @@
         <v>0</v>
       </c>
       <c r="W5">
-        <v>0</v>
+        <v>2656</v>
       </c>
       <c r="X5">
-        <v>0</v>
+        <v>2656</v>
       </c>
       <c r="Y5">
-        <v>0</v>
+        <v>2656</v>
       </c>
       <c r="Z5">
         <v>0</v>
@@ -20121,19 +20809,19 @@
         <v>0</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>1972</v>
       </c>
       <c r="Q6">
-        <v>0</v>
+        <v>1972</v>
       </c>
       <c r="R6">
-        <v>0</v>
+        <v>1972</v>
       </c>
       <c r="S6">
-        <v>0</v>
+        <v>1972</v>
       </c>
       <c r="T6">
-        <v>0</v>
+        <v>1972</v>
       </c>
       <c r="U6">
         <v>0</v>
@@ -20142,13 +20830,13 @@
         <v>0</v>
       </c>
       <c r="W6">
-        <v>0</v>
+        <v>1985</v>
       </c>
       <c r="X6">
-        <v>0</v>
+        <v>1985</v>
       </c>
       <c r="Y6">
-        <v>0</v>
+        <v>1985</v>
       </c>
       <c r="Z6">
         <v>0</v>
@@ -20675,19 +21363,19 @@
         <v>0</v>
       </c>
       <c r="P7">
-        <v>0</v>
+        <v>707</v>
       </c>
       <c r="Q7">
-        <v>0</v>
+        <v>707</v>
       </c>
       <c r="R7">
-        <v>0</v>
+        <v>707</v>
       </c>
       <c r="S7">
-        <v>0</v>
+        <v>707</v>
       </c>
       <c r="T7">
-        <v>0</v>
+        <v>707</v>
       </c>
       <c r="U7">
         <v>0</v>
@@ -20696,13 +21384,13 @@
         <v>0</v>
       </c>
       <c r="W7">
-        <v>0</v>
+        <v>549</v>
       </c>
       <c r="X7">
-        <v>0</v>
+        <v>549</v>
       </c>
       <c r="Y7">
-        <v>0</v>
+        <v>549</v>
       </c>
       <c r="Z7">
         <v>0</v>
@@ -21229,19 +21917,19 @@
         <v>0</v>
       </c>
       <c r="P8">
-        <v>0</v>
+        <v>208</v>
       </c>
       <c r="Q8">
-        <v>0</v>
+        <v>208</v>
       </c>
       <c r="R8">
-        <v>0</v>
+        <v>208</v>
       </c>
       <c r="S8">
-        <v>0</v>
+        <v>208</v>
       </c>
       <c r="T8">
-        <v>0</v>
+        <v>208</v>
       </c>
       <c r="U8">
         <v>0</v>
@@ -21250,13 +21938,13 @@
         <v>0</v>
       </c>
       <c r="W8">
-        <v>0</v>
+        <v>384</v>
       </c>
       <c r="X8">
-        <v>0</v>
+        <v>384</v>
       </c>
       <c r="Y8">
-        <v>0</v>
+        <v>384</v>
       </c>
       <c r="Z8">
         <v>0</v>
@@ -21783,19 +22471,19 @@
         <v>0</v>
       </c>
       <c r="P9">
-        <v>0</v>
+        <v>1175</v>
       </c>
       <c r="Q9">
-        <v>0</v>
+        <v>1175</v>
       </c>
       <c r="R9">
-        <v>0</v>
+        <v>1175</v>
       </c>
       <c r="S9">
-        <v>0</v>
+        <v>1175</v>
       </c>
       <c r="T9">
-        <v>0</v>
+        <v>1175</v>
       </c>
       <c r="U9">
         <v>0</v>
@@ -21804,13 +22492,13 @@
         <v>0</v>
       </c>
       <c r="W9">
-        <v>0</v>
+        <v>1185</v>
       </c>
       <c r="X9">
-        <v>0</v>
+        <v>1185</v>
       </c>
       <c r="Y9">
-        <v>0</v>
+        <v>1185</v>
       </c>
       <c r="Z9">
         <v>0</v>
@@ -22337,19 +23025,19 @@
         <v>0</v>
       </c>
       <c r="P10">
-        <v>0</v>
+        <v>3505</v>
       </c>
       <c r="Q10">
-        <v>0</v>
+        <v>3505</v>
       </c>
       <c r="R10">
-        <v>0</v>
+        <v>3505</v>
       </c>
       <c r="S10">
-        <v>0</v>
+        <v>3505</v>
       </c>
       <c r="T10">
-        <v>0</v>
+        <v>3505</v>
       </c>
       <c r="U10">
         <v>0</v>
@@ -22358,13 +23046,13 @@
         <v>0</v>
       </c>
       <c r="W10">
-        <v>0</v>
+        <v>3763</v>
       </c>
       <c r="X10">
-        <v>0</v>
+        <v>3763</v>
       </c>
       <c r="Y10">
-        <v>0</v>
+        <v>3763</v>
       </c>
       <c r="Z10">
         <v>0</v>
@@ -22891,19 +23579,19 @@
         <v>0</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="R11">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="S11">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="T11">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="U11">
         <v>0</v>
@@ -22912,13 +23600,13 @@
         <v>0</v>
       </c>
       <c r="W11">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="X11">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="Y11">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="Z11">
         <v>0</v>
@@ -23445,19 +24133,19 @@
         <v>0</v>
       </c>
       <c r="P12">
-        <v>0</v>
+        <v>376</v>
       </c>
       <c r="Q12">
-        <v>0</v>
+        <v>376</v>
       </c>
       <c r="R12">
-        <v>0</v>
+        <v>376</v>
       </c>
       <c r="S12">
-        <v>0</v>
+        <v>376</v>
       </c>
       <c r="T12">
-        <v>0</v>
+        <v>376</v>
       </c>
       <c r="U12">
         <v>0</v>
@@ -23466,13 +24154,13 @@
         <v>0</v>
       </c>
       <c r="W12">
-        <v>0</v>
+        <v>339</v>
       </c>
       <c r="X12">
-        <v>0</v>
+        <v>219</v>
       </c>
       <c r="Y12">
-        <v>0</v>
+        <v>339</v>
       </c>
       <c r="Z12">
         <v>0</v>
@@ -23999,19 +24687,19 @@
         <v>0</v>
       </c>
       <c r="P13">
-        <v>0</v>
+        <v>730</v>
       </c>
       <c r="Q13">
-        <v>0</v>
+        <v>730</v>
       </c>
       <c r="R13">
-        <v>0</v>
+        <v>730</v>
       </c>
       <c r="S13">
-        <v>0</v>
+        <v>730</v>
       </c>
       <c r="T13">
-        <v>0</v>
+        <v>730</v>
       </c>
       <c r="U13">
         <v>0</v>
@@ -24020,13 +24708,13 @@
         <v>0</v>
       </c>
       <c r="W13">
-        <v>0</v>
+        <v>730</v>
       </c>
       <c r="X13">
-        <v>0</v>
+        <v>730</v>
       </c>
       <c r="Y13">
-        <v>0</v>
+        <v>730</v>
       </c>
       <c r="Z13">
         <v>0</v>
@@ -25107,19 +25795,19 @@
         <v>0</v>
       </c>
       <c r="P15">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="Q15">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="R15">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="S15">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="T15">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="U15">
         <v>0</v>
@@ -25128,13 +25816,13 @@
         <v>0</v>
       </c>
       <c r="W15">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="X15">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="Y15">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="Z15">
         <v>0</v>
@@ -25661,19 +26349,19 @@
         <v>0</v>
       </c>
       <c r="P16">
-        <v>0</v>
+        <v>618</v>
       </c>
       <c r="Q16">
-        <v>0</v>
+        <v>618</v>
       </c>
       <c r="R16">
-        <v>0</v>
+        <v>618</v>
       </c>
       <c r="S16">
-        <v>0</v>
+        <v>618</v>
       </c>
       <c r="T16">
-        <v>0</v>
+        <v>618</v>
       </c>
       <c r="U16">
         <v>0</v>
@@ -25682,13 +26370,13 @@
         <v>0</v>
       </c>
       <c r="W16">
-        <v>0</v>
+        <v>529</v>
       </c>
       <c r="X16">
-        <v>0</v>
+        <v>529</v>
       </c>
       <c r="Y16">
-        <v>0</v>
+        <v>529</v>
       </c>
       <c r="Z16">
         <v>0</v>
@@ -26215,19 +26903,19 @@
         <v>0</v>
       </c>
       <c r="P17">
-        <v>0</v>
+        <v>3998</v>
       </c>
       <c r="Q17">
-        <v>0</v>
+        <v>3998</v>
       </c>
       <c r="R17">
-        <v>0</v>
+        <v>3998</v>
       </c>
       <c r="S17">
-        <v>0</v>
+        <v>3998</v>
       </c>
       <c r="T17">
-        <v>0</v>
+        <v>3998</v>
       </c>
       <c r="U17">
         <v>0</v>
@@ -26236,13 +26924,13 @@
         <v>0</v>
       </c>
       <c r="W17">
-        <v>0</v>
+        <v>3998</v>
       </c>
       <c r="X17">
-        <v>0</v>
+        <v>3998</v>
       </c>
       <c r="Y17">
-        <v>0</v>
+        <v>3998</v>
       </c>
       <c r="Z17">
         <v>0</v>
@@ -26769,19 +27457,19 @@
         <v>0</v>
       </c>
       <c r="P18">
-        <v>0</v>
+        <v>913</v>
       </c>
       <c r="Q18">
-        <v>0</v>
+        <v>1173</v>
       </c>
       <c r="R18">
-        <v>0</v>
+        <v>1173</v>
       </c>
       <c r="S18">
-        <v>0</v>
+        <v>1173</v>
       </c>
       <c r="T18">
-        <v>0</v>
+        <v>1173</v>
       </c>
       <c r="U18">
         <v>0</v>
@@ -26790,13 +27478,13 @@
         <v>0</v>
       </c>
       <c r="W18">
-        <v>0</v>
+        <v>1173</v>
       </c>
       <c r="X18">
-        <v>0</v>
+        <v>1173</v>
       </c>
       <c r="Y18">
-        <v>0</v>
+        <v>1173</v>
       </c>
       <c r="Z18">
         <v>0</v>
@@ -27323,19 +28011,19 @@
         <v>0</v>
       </c>
       <c r="P19">
-        <v>0</v>
+        <v>219</v>
       </c>
       <c r="Q19">
-        <v>0</v>
+        <v>219</v>
       </c>
       <c r="R19">
-        <v>0</v>
+        <v>219</v>
       </c>
       <c r="S19">
-        <v>0</v>
+        <v>219</v>
       </c>
       <c r="T19">
-        <v>0</v>
+        <v>219</v>
       </c>
       <c r="U19">
         <v>0</v>
@@ -27344,13 +28032,13 @@
         <v>0</v>
       </c>
       <c r="W19">
-        <v>0</v>
+        <v>424</v>
       </c>
       <c r="X19">
-        <v>0</v>
+        <v>424</v>
       </c>
       <c r="Y19">
-        <v>0</v>
+        <v>424</v>
       </c>
       <c r="Z19">
         <v>0</v>
@@ -27877,19 +28565,19 @@
         <v>0</v>
       </c>
       <c r="P20">
-        <v>0</v>
+        <v>408</v>
       </c>
       <c r="Q20">
-        <v>0</v>
+        <v>408</v>
       </c>
       <c r="R20">
-        <v>0</v>
+        <v>408</v>
       </c>
       <c r="S20">
-        <v>0</v>
+        <v>408</v>
       </c>
       <c r="T20">
-        <v>0</v>
+        <v>408</v>
       </c>
       <c r="U20">
         <v>0</v>
@@ -27898,13 +28586,13 @@
         <v>0</v>
       </c>
       <c r="W20">
-        <v>0</v>
+        <v>408</v>
       </c>
       <c r="X20">
-        <v>0</v>
+        <v>408</v>
       </c>
       <c r="Y20">
-        <v>0</v>
+        <v>408</v>
       </c>
       <c r="Z20">
         <v>0</v>
@@ -28431,19 +29119,19 @@
         <v>0</v>
       </c>
       <c r="P21">
-        <v>0</v>
+        <v>203</v>
       </c>
       <c r="Q21">
-        <v>0</v>
+        <v>203</v>
       </c>
       <c r="R21">
-        <v>0</v>
+        <v>203</v>
       </c>
       <c r="S21">
-        <v>0</v>
+        <v>203</v>
       </c>
       <c r="T21">
-        <v>0</v>
+        <v>203</v>
       </c>
       <c r="U21">
         <v>0</v>
@@ -28452,13 +29140,13 @@
         <v>0</v>
       </c>
       <c r="W21">
-        <v>0</v>
+        <v>305</v>
       </c>
       <c r="X21">
-        <v>0</v>
+        <v>305</v>
       </c>
       <c r="Y21">
-        <v>0</v>
+        <v>305</v>
       </c>
       <c r="Z21">
         <v>0</v>
@@ -28985,19 +29673,19 @@
         <v>0</v>
       </c>
       <c r="P22">
-        <v>0</v>
+        <v>3604</v>
       </c>
       <c r="Q22">
-        <v>0</v>
+        <v>4114</v>
       </c>
       <c r="R22">
-        <v>0</v>
+        <v>4114</v>
       </c>
       <c r="S22">
-        <v>0</v>
+        <v>4114</v>
       </c>
       <c r="T22">
-        <v>0</v>
+        <v>4114</v>
       </c>
       <c r="U22">
         <v>0</v>
@@ -29006,13 +29694,13 @@
         <v>0</v>
       </c>
       <c r="W22">
-        <v>0</v>
+        <v>4198</v>
       </c>
       <c r="X22">
-        <v>0</v>
+        <v>4198</v>
       </c>
       <c r="Y22">
-        <v>0</v>
+        <v>4198</v>
       </c>
       <c r="Z22">
         <v>0</v>

</xml_diff>

<commit_message>
PVS: switch to WH Receipt workbook for planned data, remove Excel COM dependency, refine table styling and header colors
</commit_message>
<xml_diff>
--- a/PVS/Planned_qtys.xlsx
+++ b/PVS/Planned_qtys.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Logistics\4_BSA\9_Scripts_Reports\Daily_Production_IT\PVS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C05541C-9313-4C9A-AB7D-468958A7B0C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363E6478-FE2A-40F2-9798-D791990ACC1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{86600EFC-FD9C-43BB-B6BA-9F2124CEAC73}"/>
   </bookViews>
@@ -17736,7 +17736,7 @@
   <dimension ref="A1:PL22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>